<commit_message>
New translations multilingual_spreadsheet_sample.xlsx (Multilingual)
</commit_message>
<xml_diff>
--- a/fr/Multilingual_spreadsheet_sample.xlsx
+++ b/fr/Multilingual_spreadsheet_sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Key</t>
   </si>
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -522,8 +522,11 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -539,8 +542,11 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -556,8 +562,11 @@
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -573,8 +582,11 @@
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -588,6 +600,9 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>